<commit_message>
add color code to general template
</commit_message>
<xml_diff>
--- a/data-raw/New general trust template.xlsx
+++ b/data-raw/New general trust template.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F6D3724-B786-E748-9A2A-CC714F02CFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Git_version\experiencesdashboard\data-raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DD31FC-0B18-4FB7-8482-E8F6464351C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15915" yWindow="3060" windowWidth="15180" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>date</t>
   </si>
@@ -139,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,16 +159,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -171,17 +196,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,73 +540,73 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.4375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="34.4375" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="14.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44469</v>
       </c>
@@ -611,7 +651,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44861</v>
       </c>

</xml_diff>